<commit_message>
liftclaw and teleop changes
</commit_message>
<xml_diff>
--- a/Calculators/DriveCalculators.xlsx
+++ b/Calculators/DriveCalculators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gweaver/Documents/GitHub/2023CompetitionCode/Calculators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28265903-7675-194A-8C4D-21D76C228538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BE6318-52A3-8A43-BE07-751FA247A7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{10FBA7F1-CCF1-468D-B0AD-B0C42B5651D8}"/>
+    <workbookView xWindow="1320" yWindow="940" windowWidth="27620" windowHeight="16660" xr2:uid="{10FBA7F1-CCF1-468D-B0AD-B0C42B5651D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>